<commit_message>
add import class function
</commit_message>
<xml_diff>
--- a/class.xlsx
+++ b/class.xlsx
@@ -35,9 +35,6 @@
     <t>Pupil SurName</t>
   </si>
   <si>
-    <t>Pupil Class</t>
-  </si>
-  <si>
     <t>Parent Email</t>
   </si>
   <si>
@@ -59,16 +56,19 @@
     <t>Parent SurName</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>bbb</t>
-  </si>
-  <si>
-    <t>ccc</t>
-  </si>
-  <si>
-    <t>ddd</t>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Mason</t>
+  </si>
+  <si>
+    <t>Cater</t>
+  </si>
+  <si>
+    <t>Jackson</t>
   </si>
 </sst>
 </file>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,27 +445,27 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -485,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>

</xml_diff>